<commit_message>
custom server room full
</commit_message>
<xml_diff>
--- a/RTC Documents/성능 테스트.xlsx
+++ b/RTC Documents/성능 테스트.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lee\study\Test-WebRtc\RTC MultiConnection\proto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lee\study\Test-WebRtc\RTC Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53B1041D-A072-4149-92A3-816D795E01F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9668F561-B35C-4EA8-BA73-4D6B5DCBAB1D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B999A838-1D08-4BBF-A85E-569F8CFFA738}"/>
+    <workbookView xWindow="4005" yWindow="2370" windowWidth="21585" windowHeight="11370" xr2:uid="{B999A838-1D08-4BBF-A85E-569F8CFFA738}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="37">
   <si>
     <t>Fire Fox</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +140,41 @@
   </si>
   <si>
     <t>extantion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>License</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BSD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>coturnAPI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rmcAPI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MIT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ffmpeg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LGPL</t>
+  </si>
+  <si>
+    <t>SSL인증</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OpenSSL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -147,7 +182,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +197,12 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF545454"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,12 +227,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -507,333 +551,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C998AB3B-3CE7-43CD-B034-BC71B811CA97}">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:N31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="C1" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1"/>
+      <c r="M1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="D4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="E4" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="F4" t="s">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="G4" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="I4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="C9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="1" t="s">
+      <c r="B10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="D10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="D11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1">
+      <c r="B12" s="1">
         <v>5</v>
       </c>
-      <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="D16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
@@ -841,7 +886,6 @@
       <c r="G17" s="1"/>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
@@ -849,7 +893,6 @@
       <c r="G18" s="1"/>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
@@ -857,7 +900,6 @@
       <c r="G19" s="1"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>

</xml_diff>